<commit_message>
removed RIN column from rnaSample 08.12.19
</commit_message>
<xml_diff>
--- a/library/Library_BrownH_12.19.19.xlsx
+++ b/library/Library_BrownH_12.19.19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DB081F-3744-1A4C-B4D8-A1C43534A21B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA7AB5A-58AA-B244-85B9-095763881DD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27200" windowHeight="14920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7620" yWindow="1920" windowWidth="27200" windowHeight="14920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -244,9 +244,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -311,7 +308,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,7 +626,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G27"/>
+      <selection activeCell="L2" sqref="L2:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,7 +723,6 @@
         <v>17</v>
       </c>
       <c r="L2" s="6" t="b">
-        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="M2" s="1"/>

</xml_diff>